<commit_message>
Added bowler source files to try and compare old process with new process. Counts aren't matching active and terminated report or 1/1/24 effective dated reports.
</commit_message>
<xml_diff>
--- a/outputs/internal_fill_test.xlsx
+++ b/outputs/internal_fill_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://regalrexnord-my.sharepoint.com/personal/jenna_eagleson_regalrexnord_com/Documents/Documents/2024/2024_Core Value Drivers_Reporting/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_2AE941EECBA7E8EA43EDFE8C5080F63CAB6A4398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3228049-A995-490B-B847-F1EF077CDE24}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_2AE941EECBA7E8EA43EDFE8C5080F63CAB6A4398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B1BE34-DE79-427E-9A83-B1F58F60A0F4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="all_data" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">all_data!$A$1:$AR$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">all_data!$A$1:$AR$110</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -3003,7 +3003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -3317,7 +3319,7 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15864,7 +15866,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AR1" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WAHOOO - working as expected!
</commit_message>
<xml_diff>
--- a/outputs/internal_fill_test.xlsx
+++ b/outputs/internal_fill_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://regalrexnord-my.sharepoint.com/personal/jenna_eagleson_regalrexnord_com/Documents/Documents/2024/2024_Core Value Drivers_Reporting/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_2AE941EECBA7E8EA43EDFE8C5080F63CAB6A4398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B1BE34-DE79-427E-9A83-B1F58F60A0F4}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_2AE941EECBA7E8EA43EDFE8C5080F63CAB6A4398" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AD03DAB-6D7A-423D-B134-E9A34B474F13}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enterprise" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,23 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">all_data!$A$1:$AR$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">by_segment_level!$A$1:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">by_segment_location!$A$1:$F$58</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2850,7 +2865,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2908,6 +2925,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -3001,13 +3021,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -3049,7 +3076,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -3089,7 +3116,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3109,7 +3136,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3129,7 +3156,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3149,7 +3176,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3169,7 +3196,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3189,7 +3216,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3209,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3229,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3249,7 +3276,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3310,19 +3337,31 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F15" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Industrial Powertrain Solutions (IPS)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -3364,7 +3403,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3384,7 +3423,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3404,7 +3443,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3424,7 +3463,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3444,7 +3483,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -3464,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3484,7 +3523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3504,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3524,7 +3563,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3544,7 +3583,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3564,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3664,7 +3703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3684,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -3704,7 +3743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -3724,7 +3763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -3744,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -3764,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -3784,7 +3823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -3804,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -3824,7 +3863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -3844,7 +3883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -3864,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -3884,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -3904,7 +3943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -3924,7 +3963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -3944,7 +3983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -3964,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -3984,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -4004,7 +4043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -4304,7 +4343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -4324,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -4344,7 +4383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -4364,7 +4403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -4384,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -4404,7 +4443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -4424,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -4444,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -4464,7 +4503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -4485,21 +4524,36 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F58" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Industrial Powertrain Solutions (IPS)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AR110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="40" customWidth="1"/>
     <col min="5" max="5" width="20.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" style="2" customWidth="1"/>
     <col min="10" max="10" width="20.7265625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="59.7265625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="20.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4637,7 +4691,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -4708,7 +4762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -4779,7 +4833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -4850,7 +4904,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>133</v>
       </c>
@@ -4921,7 +4975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -5406,7 +5460,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>203</v>
       </c>
@@ -5528,7 +5582,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>216</v>
       </c>
@@ -5772,7 +5826,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>236</v>
       </c>
@@ -6013,7 +6067,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>246</v>
       </c>
@@ -6084,7 +6138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>249</v>
       </c>
@@ -6203,7 +6257,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>255</v>
       </c>
@@ -6325,7 +6379,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -6396,7 +6450,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>272</v>
       </c>
@@ -6515,7 +6569,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>281</v>
       </c>
@@ -6637,7 +6691,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>293</v>
       </c>
@@ -6759,7 +6813,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>299</v>
       </c>
@@ -6830,7 +6884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>301</v>
       </c>
@@ -6901,7 +6955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>303</v>
       </c>
@@ -7023,7 +7077,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>305</v>
       </c>
@@ -7094,7 +7148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>314</v>
       </c>
@@ -7165,7 +7219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>316</v>
       </c>
@@ -7287,7 +7341,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>320</v>
       </c>
@@ -7358,7 +7412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>322</v>
       </c>
@@ -7480,7 +7534,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>334</v>
       </c>
@@ -7551,7 +7605,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>336</v>
       </c>
@@ -7670,7 +7724,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>346</v>
       </c>
@@ -7789,7 +7843,7 @@
         <v>45679</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>355</v>
       </c>
@@ -7911,7 +7965,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>365</v>
       </c>
@@ -7982,7 +8036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>374</v>
       </c>
@@ -8053,7 +8107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>376</v>
       </c>
@@ -8175,7 +8229,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>385</v>
       </c>
@@ -8294,7 +8348,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>400</v>
       </c>
@@ -8660,7 +8714,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>421</v>
       </c>
@@ -8782,7 +8836,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>429</v>
       </c>
@@ -8916,7 +8970,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>436</v>
       </c>
@@ -9038,7 +9092,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>445</v>
       </c>
@@ -9160,7 +9214,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>452</v>
       </c>
@@ -9282,7 +9336,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>460</v>
       </c>
@@ -9404,7 +9458,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>466</v>
       </c>
@@ -9526,7 +9580,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>472</v>
       </c>
@@ -9645,7 +9699,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>478</v>
       </c>
@@ -9716,7 +9770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>484</v>
       </c>
@@ -9799,7 +9853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>491</v>
       </c>
@@ -9921,7 +9975,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>497</v>
       </c>
@@ -9992,7 +10046,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>500</v>
       </c>
@@ -10114,7 +10168,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>505</v>
       </c>
@@ -10236,7 +10290,7 @@
         <v>45664</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>511</v>
       </c>
@@ -10307,7 +10361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>516</v>
       </c>
@@ -10429,7 +10483,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>523</v>
       </c>
@@ -10500,7 +10554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>527</v>
       </c>
@@ -10571,7 +10625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>531</v>
       </c>
@@ -10693,7 +10747,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>540</v>
       </c>
@@ -10764,7 +10818,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>547</v>
       </c>
@@ -10868,7 +10922,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>554</v>
       </c>
@@ -10972,7 +11026,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>563</v>
       </c>
@@ -11076,7 +11130,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>569</v>
       </c>
@@ -11180,7 +11234,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>579</v>
       </c>
@@ -11284,7 +11338,7 @@
         <v>45659</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>586</v>
       </c>
@@ -11388,7 +11442,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>594</v>
       </c>
@@ -11492,7 +11546,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>599</v>
       </c>
@@ -11596,7 +11650,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>604</v>
       </c>
@@ -11700,7 +11754,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>612</v>
       </c>
@@ -11804,7 +11858,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>617</v>
       </c>
@@ -11908,7 +11962,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>624</v>
       </c>
@@ -12012,7 +12066,7 @@
         <v>45664</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>630</v>
       </c>
@@ -12116,7 +12170,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>635</v>
       </c>
@@ -12220,7 +12274,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>639</v>
       </c>
@@ -12324,7 +12378,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>649</v>
       </c>
@@ -12428,7 +12482,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>656</v>
       </c>
@@ -12532,7 +12586,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>658</v>
       </c>
@@ -12636,7 +12690,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>661</v>
       </c>
@@ -12740,7 +12794,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>664</v>
       </c>
@@ -12844,7 +12898,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>666</v>
       </c>
@@ -12948,7 +13002,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>671</v>
       </c>
@@ -13052,7 +13106,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>673</v>
       </c>
@@ -13156,7 +13210,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>677</v>
       </c>
@@ -13260,7 +13314,7 @@
         <v>45663</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>681</v>
       </c>
@@ -13364,7 +13418,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>686</v>
       </c>
@@ -13468,7 +13522,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>691</v>
       </c>
@@ -13572,7 +13626,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>696</v>
       </c>
@@ -13676,7 +13730,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>699</v>
       </c>
@@ -13780,7 +13834,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>705</v>
       </c>
@@ -13884,7 +13938,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>711</v>
       </c>
@@ -13988,7 +14042,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>715</v>
       </c>
@@ -14092,7 +14146,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>720</v>
       </c>
@@ -14196,7 +14250,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>728</v>
       </c>
@@ -14300,7 +14354,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>731</v>
       </c>
@@ -14404,7 +14458,7 @@
         <v>45672</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>738</v>
       </c>
@@ -14508,7 +14562,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>743</v>
       </c>
@@ -14612,7 +14666,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>747</v>
       </c>
@@ -14716,7 +14770,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>749</v>
       </c>
@@ -14820,7 +14874,7 @@
         <v>45670</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>754</v>
       </c>
@@ -14924,7 +14978,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>758</v>
       </c>
@@ -15028,7 +15082,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>765</v>
       </c>
@@ -15132,7 +15186,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>769</v>
       </c>
@@ -15236,7 +15290,7 @@
         <v>45677</v>
       </c>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>773</v>
       </c>
@@ -15340,7 +15394,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>780</v>
       </c>
@@ -15444,7 +15498,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>785</v>
       </c>
@@ -15548,7 +15602,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>790</v>
       </c>
@@ -15652,7 +15706,7 @@
         <v>45684</v>
       </c>
     </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>795</v>
       </c>
@@ -15723,7 +15777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>800</v>
       </c>
@@ -15794,7 +15848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:44" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>806</v>
       </c>
@@ -15866,6 +15920,23 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AR110" xr:uid="{00000000-0001-0000-0400-000000000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="Milwaukee Pmc Hq Wisconsin"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="15">
+      <filters>
+        <filter val="Industrial Powertrain Solutions (IPS)"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="25">
+      <filters>
+        <filter val="Internal"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>